<commit_message>
Updated workflow and api_docs
</commit_message>
<xml_diff>
--- a/src/test/resources/api_document/dev_api_doc.xlsx
+++ b/src/test/resources/api_document/dev_api_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\IdeaProjects\MaxSoft-IntelliAPI\src\test\resources\api_document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0A3469-B382-4751-AD62-B60F628DE2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D74317-6C52-4F52-A429-49ADC2079E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>API_NAME</t>
   </si>
@@ -164,9 +164,9 @@
     <t>http://8e4jz.mocklab.io/tasks</t>
   </si>
   <si>
-    <t xml:space="preserve">{                         
+    <t>{                         
   "app" : "#app"                                 
-}  </t>
+}</t>
   </si>
 </sst>
 </file>
@@ -1538,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1761,20 +1761,22 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
     </row>
-    <row r="11" spans="1:20" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1817,25 +1819,8 @@
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1845,13 +1830,12 @@
     <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B9" r:id="rId5" xr:uid="{EF72D20A-29EB-4276-97F0-89696C6AEFB9}"/>
     <hyperlink ref="B6:B8" r:id="rId6" display="https://gorest.co.in/public-api/users" xr:uid="{E4541788-CF20-4394-9324-49724D2E3050}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{71384265-6436-442A-BCD1-873C3299A30B}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{E8E3651D-5CE1-4081-959D-1BA97F111FB2}"/>
-    <hyperlink ref="B13" r:id="rId9" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
-    <hyperlink ref="B14" r:id="rId10" xr:uid="{EFEF718E-7793-46D0-81EC-9B04EBE89157}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{E8E3651D-5CE1-4081-959D-1BA97F111FB2}"/>
+    <hyperlink ref="B13" r:id="rId8" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{BABD2832-B84B-4B58-AC15-D3B05C9DA314}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added more header related tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/api_document/dev_api_doc.xlsx
+++ b/src/test/resources/api_document/dev_api_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\IdeaProjects\MaxSoft-IntelliAPI\src\test\resources\api_document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941232F3-43B9-48F9-8813-B15B5B6218F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74D348C-8026-4B2E-9E18-D3523CA9A292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>API_NAME</t>
   </si>
@@ -155,18 +155,27 @@
     <t>https://api.apis.guru/#version/#jsonFile</t>
   </si>
   <si>
-    <t>Create task</t>
-  </si>
-  <si>
-    <t>http://8e4jz.mocklab.io/tasks</t>
-  </si>
-  <si>
-    <t>{                         
-  "app" : "#app"                                 
+    <t>https://intelliapi-mockserver.herokuapp.com/auth</t>
+  </si>
+  <si>
+    <t>Get all tasks</t>
+  </si>
+  <si>
+    <t>https://intelliapi-mockserver.herokuapp.com/tasks</t>
+  </si>
+  <si>
+    <t>Create a task</t>
+  </si>
+  <si>
+    <t>{
+    "status": [
+        "#status"
+    ],
+    "name": "#name",
+    "category": "#category",
+    "isDeleted": #isDeleted,
+    "__v": #version
 }</t>
-  </si>
-  <si>
-    <t>https://intelliapi-mockserver.herokuapp.com/auth</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1550,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1584,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -1761,12 +1770,12 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
     </row>
-    <row r="11" spans="1:20" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="13" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>4</v>
@@ -1775,7 +1784,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1819,6 +1828,19 @@
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
     </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+    </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
     </row>
@@ -1833,9 +1855,10 @@
     <hyperlink ref="B12" r:id="rId7" xr:uid="{E8E3651D-5CE1-4081-959D-1BA97F111FB2}"/>
     <hyperlink ref="B13" r:id="rId8" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
     <hyperlink ref="B11" r:id="rId9" xr:uid="{BABD2832-B84B-4B58-AC15-D3B05C9DA314}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{3E3D4B4F-3617-4625-8089-C2EE3F74B53E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Implemented steps to invoke GET API from data store values
</commit_message>
<xml_diff>
--- a/src/test/resources/api_document/dev_api_doc.xlsx
+++ b/src/test/resources/api_document/dev_api_doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\IdeaProjects\MaxSoft-IntelliAPI\src\test\resources\api_document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74D348C-8026-4B2E-9E18-D3523CA9A292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C6B9A-E355-40B5-86A3-7EF239F96E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_Template" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>API_NAME</t>
   </si>
@@ -176,6 +176,12 @@
     "isDeleted": #isDeleted,
     "__v": #version
 }</t>
+  </si>
+  <si>
+    <t>Get urls</t>
+  </si>
+  <si>
+    <t>https://intelliapi-mockserver.herokuapp.com/photos</t>
   </si>
 </sst>
 </file>
@@ -1549,20 +1555,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" style="1" customWidth="1"/>
-    <col min="6" max="20" width="8.85546875" style="12"/>
+    <col min="1" max="1" width="61.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="1" customWidth="1"/>
+    <col min="6" max="20" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1592,7 +1598,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>36</v>
       </c>
@@ -1622,7 +1628,7 @@
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
     </row>
-    <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
@@ -1637,7 +1643,7 @@
       </c>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="1:20" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1688,7 @@
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
     </row>
-    <row r="7" spans="1:20" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -1727,7 +1733,7 @@
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
     </row>
-    <row r="9" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
@@ -1740,7 +1746,7 @@
       <c r="D9" s="10"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:20" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -1770,7 +1776,7 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
     </row>
-    <row r="11" spans="1:20" s="13" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="13" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>45</v>
       </c>
@@ -1802,7 +1808,7 @@
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
     </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>40</v>
       </c>
@@ -1815,7 +1821,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>39</v>
       </c>
@@ -1828,7 +1834,7 @@
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>43</v>
       </c>
@@ -1841,7 +1847,20 @@
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
     </row>
   </sheetData>
@@ -1856,9 +1875,10 @@
     <hyperlink ref="B13" r:id="rId8" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
     <hyperlink ref="B11" r:id="rId9" xr:uid="{BABD2832-B84B-4B58-AC15-D3B05C9DA314}"/>
     <hyperlink ref="B14" r:id="rId10" xr:uid="{3E3D4B4F-3617-4625-8089-C2EE3F74B53E}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{8D01136C-9B08-4183-B697-8247C476B922}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1873,13 +1893,13 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1895,7 +1915,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1916,13 +1936,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1938,7 +1958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1946,7 +1966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -1954,7 +1974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
PATCH request implemented | Code refactored
</commit_message>
<xml_diff>
--- a/src/test/resources/api_document/dev_api_doc.xlsx
+++ b/src/test/resources/api_document/dev_api_doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\IdeaProjects\MaxSoft-IntelliAPI\src\test\resources\api_document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C6B9A-E355-40B5-86A3-7EF239F96E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D225BE-3D0F-4400-B504-930F4115C98A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_Template" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>API_NAME</t>
   </si>
@@ -182,6 +182,27 @@
   </si>
   <si>
     <t>https://intelliapi-mockserver.herokuapp.com/photos</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Edit a user (PATCH)</t>
+  </si>
+  <si>
+    <t>{
+        "name": "#name",
+        "email": "#email"
+}</t>
+  </si>
+  <si>
+    <t>Edit a task (PATCH)</t>
+  </si>
+  <si>
+    <t>{
+    "name": "#name",
+    "category": "#category"
+}</t>
   </si>
 </sst>
 </file>
@@ -221,7 +242,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,12 +258,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDBE5F1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,9 +311,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -320,14 +332,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1553,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1565,7 +1580,7 @@
     <col min="2" max="2" width="52.33203125" style="2" customWidth="1"/>
     <col min="3" max="4" width="14.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="56.6640625" style="1" customWidth="1"/>
-    <col min="6" max="20" width="8.88671875" style="12"/>
+    <col min="6" max="20" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1585,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1598,69 +1613,69 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-    </row>
-    <row r="4" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E3" s="15"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:20" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:20" s="11" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -1672,196 +1687,260 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-    </row>
-    <row r="7" spans="1:20" s="12" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+    </row>
+    <row r="7" spans="1:20" s="11" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-    </row>
-    <row r="9" spans="1:20" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+    </row>
+    <row r="10" spans="1:20" s="11" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:20" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:20" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-    </row>
-    <row r="11" spans="1:20" s="13" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" s="12" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B17" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1869,16 +1948,18 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{EF72D20A-29EB-4276-97F0-89696C6AEFB9}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{EF72D20A-29EB-4276-97F0-89696C6AEFB9}"/>
     <hyperlink ref="B6:B8" r:id="rId6" display="https://gorest.co.in/public-api/users" xr:uid="{E4541788-CF20-4394-9324-49724D2E3050}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{E8E3651D-5CE1-4081-959D-1BA97F111FB2}"/>
-    <hyperlink ref="B13" r:id="rId8" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{BABD2832-B84B-4B58-AC15-D3B05C9DA314}"/>
-    <hyperlink ref="B14" r:id="rId10" xr:uid="{3E3D4B4F-3617-4625-8089-C2EE3F74B53E}"/>
-    <hyperlink ref="B15" r:id="rId11" xr:uid="{8D01136C-9B08-4183-B697-8247C476B922}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{E8E3651D-5CE1-4081-959D-1BA97F111FB2}"/>
+    <hyperlink ref="B15" r:id="rId8" location="version/#jsonFile" xr:uid="{F2C53B19-03F4-440A-8B1D-9B452BFD966E}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{BABD2832-B84B-4B58-AC15-D3B05C9DA314}"/>
+    <hyperlink ref="B16" r:id="rId10" xr:uid="{3E3D4B4F-3617-4625-8089-C2EE3F74B53E}"/>
+    <hyperlink ref="B17" r:id="rId11" xr:uid="{8D01136C-9B08-4183-B697-8247C476B922}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{0EF4B8B6-C90E-4D48-B304-F2C83034E173}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{016831A9-122C-47FD-B9A1-8AC9BB054CB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1975,10 +2056,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>